<commit_message>
"Quang Linh gộp code lại rồi nè "
</commit_message>
<xml_diff>
--- a/excel/DanhSachCTPhieuMuon.xlsx
+++ b/excel/DanhSachCTPhieuMuon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="20">
   <si>
     <t>MaPM</t>
   </si>
@@ -116,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -509,13 +509,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -523,10 +523,10 @@
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
@@ -534,9 +534,20 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>